<commit_message>
Substrates added to kinetics in ontology
</commit_message>
<xml_diff>
--- a/Abbaspour/ELNs/New-ELN_Kinetik_1.xlsx
+++ b/Abbaspour/ELNs/New-ELN_Kinetik_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Abschlussarbeiten_Behr\Abbaspour\ELNs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1606B04D-6759-4FDC-A552-4EA3D3340209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAE1E26-9640-41F4-84DD-1F8C0B54D8E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33225" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Substances and Reactions" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="182">
   <si>
     <t>Laccase</t>
   </si>
@@ -577,9 +577,6 @@
   </si>
   <si>
     <t>baseCompound</t>
-  </si>
-  <si>
-    <t>ABTS_red, Oxygen, Water</t>
   </si>
 </sst>
 </file>
@@ -1259,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,7 +1557,7 @@
         <v>181</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>182</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>